<commit_message>
invisibility on ranger works
</commit_message>
<xml_diff>
--- a/Documentation/Classes and Skills.xlsx
+++ b/Documentation/Classes and Skills.xlsx
@@ -601,7 +601,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -793,7 +793,7 @@
         <v>9</v>
       </c>
       <c r="H9">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="J9" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
added berserker rage to warrior 2
</commit_message>
<xml_diff>
--- a/Documentation/Classes and Skills.xlsx
+++ b/Documentation/Classes and Skills.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>Warrior</t>
   </si>
@@ -117,9 +117,6 @@
     <t>fov calculations off and maybe grey shader</t>
   </si>
   <si>
-    <t>increased attack speed (lower timebetweenattacks) and increased dmg for some time + red shader</t>
-  </si>
-  <si>
     <t>drops trap that makes enemy frozen</t>
   </si>
   <si>
@@ -181,6 +178,12 @@
   </si>
   <si>
     <t>teleport in any direction with max 5 cells distance</t>
+  </si>
+  <si>
+    <t>increased attack speed (lower timebetweenattacks) + lifesteal + red shader</t>
+  </si>
+  <si>
+    <t>lasts 10s</t>
   </si>
 </sst>
 </file>
@@ -601,7 +604,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,7 +621,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>0</v>
@@ -662,7 +665,7 @@
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J2" t="s">
         <v>29</v>
@@ -711,7 +714,7 @@
         <v>30</v>
       </c>
       <c r="J4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -733,8 +736,11 @@
       <c r="H5">
         <v>10</v>
       </c>
+      <c r="I5" t="s">
+        <v>55</v>
+      </c>
       <c r="J5" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -768,10 +774,10 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -782,12 +788,12 @@
         <v>30</v>
       </c>
       <c r="J8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>9</v>
@@ -804,7 +810,7 @@
         <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>27</v>
@@ -816,18 +822,18 @@
         <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>20</v>
@@ -836,18 +842,18 @@
         <v>30</v>
       </c>
       <c r="J11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>12</v>
@@ -856,18 +862,18 @@
         <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>19</v>
@@ -876,7 +882,7 @@
         <v>60</v>
       </c>
       <c r="J13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -887,7 +893,7 @@
         <v>60</v>
       </c>
       <c r="J14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -898,7 +904,7 @@
         <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -909,7 +915,7 @@
         <v>100</v>
       </c>
       <c r="J16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added frost nova spell (mage 2)
</commit_message>
<xml_diff>
--- a/Documentation/Classes and Skills.xlsx
+++ b/Documentation/Classes and Skills.xlsx
@@ -603,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -901,7 +901,7 @@
         <v>13</v>
       </c>
       <c r="H15">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="J15" t="s">
         <v>36</v>

</xml_diff>